<commit_message>
care insurance test cases
</commit_message>
<xml_diff>
--- a/src/test/java/com/xpresso/qa/testdata/Xpresso_TestData.xlsx
+++ b/src/test/java/com/xpresso/qa/testdata/Xpresso_TestData.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F371F5A7-1A03-47EF-B248-2C83B89156C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rohit.mathur\RoinetGit\XpressoTestingGit\src\test\java\com\xpresso\qa\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CAAC38-B97B-4889-A0F4-3AA667E02C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Channel" sheetId="1" r:id="rId1"/>
     <sheet name="Wallet" sheetId="2" r:id="rId2"/>
-    <sheet name="Services" sheetId="3" r:id="rId3"/>
+    <sheet name="CareInsurance" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:K5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="98">
   <si>
     <t>Name</t>
   </si>
@@ -89,6 +93,234 @@
   </si>
   <si>
     <t>InValid</t>
+  </si>
+  <si>
+    <t>coverType</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>sinsure</t>
+  </si>
+  <si>
+    <t>50K</t>
+  </si>
+  <si>
+    <t>nRelation</t>
+  </si>
+  <si>
+    <t>MOTHER</t>
+  </si>
+  <si>
+    <t>numberOfMembers</t>
+  </si>
+  <si>
+    <t>editNumberMember</t>
+  </si>
+  <si>
+    <t>numberOfMembersCompare</t>
+  </si>
+  <si>
+    <t>InsuPeriod</t>
+  </si>
+  <si>
+    <t>1Y</t>
+  </si>
+  <si>
+    <t>insuPeriodCompare</t>
+  </si>
+  <si>
+    <t>InsuProduct</t>
+  </si>
+  <si>
+    <t>Group Care 360°(ROINET)-GMC</t>
+  </si>
+  <si>
+    <t>InsuType</t>
+  </si>
+  <si>
+    <t>Health Insurance</t>
+  </si>
+  <si>
+    <t>nomineeName</t>
+  </si>
+  <si>
+    <t>Rohit</t>
+  </si>
+  <si>
+    <t>nomineeRelation</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>fname</t>
+  </si>
+  <si>
+    <t>iyu</t>
+  </si>
+  <si>
+    <t>lname</t>
+  </si>
+  <si>
+    <t>trtyt</t>
+  </si>
+  <si>
+    <t>gend</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>genderDB</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>rel</t>
+  </si>
+  <si>
+    <t>SELF</t>
+  </si>
+  <si>
+    <t>tit</t>
+  </si>
+  <si>
+    <t>Mr.</t>
+  </si>
+  <si>
+    <t>add1</t>
+  </si>
+  <si>
+    <t>poipoo ouwep pipi pi</t>
+  </si>
+  <si>
+    <t>add2</t>
+  </si>
+  <si>
+    <t>trteyr erwerwiiu uiuiuiui</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>trte rtertert rtrwwwt</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>DELHI &amp;</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Gurgaon</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>propEmail</t>
+  </si>
+  <si>
+    <t>pouipi@cwewrc.in</t>
+  </si>
+  <si>
+    <t>stateCompare</t>
+  </si>
+  <si>
+    <t>DELHI &amp; NCR</t>
+  </si>
+  <si>
+    <t>spouseyear</t>
+  </si>
+  <si>
+    <t>spousemonth</t>
+  </si>
+  <si>
+    <t>spousedate</t>
+  </si>
+  <si>
+    <t>childyear</t>
+  </si>
+  <si>
+    <t>childmonth</t>
+  </si>
+  <si>
+    <t>childdate</t>
+  </si>
+  <si>
+    <t>spousegend</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>spouserel</t>
+  </si>
+  <si>
+    <t>Spouse</t>
+  </si>
+  <si>
+    <t>spousetit</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>childgend</t>
+  </si>
+  <si>
+    <t>childrel</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>childtit</t>
+  </si>
+  <si>
+    <t>proposerpermanentadd1</t>
+  </si>
+  <si>
+    <t>IOIU IOY YR IO UP</t>
+  </si>
+  <si>
+    <t>proposerpermanentadd2</t>
+  </si>
+  <si>
+    <t>ATER IOAYUEUW POQ TU</t>
+  </si>
+  <si>
+    <t>proposerpermanentarea</t>
+  </si>
+  <si>
+    <t>IOY IOUPIO UPOAR</t>
+  </si>
+  <si>
+    <t>proposerpermanentstate</t>
+  </si>
+  <si>
+    <t>proposerpermanentcity</t>
+  </si>
+  <si>
+    <t>proposerpermanentpincode</t>
+  </si>
+  <si>
+    <t>proposerEmail</t>
   </si>
 </sst>
 </file>
@@ -409,7 +641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -617,14 +849,402 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9D1BA2-6B7F-4E24-A24E-7F425DA68E7E}">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>67</v>
+      </c>
+      <c r="B28">
+        <v>122012</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>73</v>
+      </c>
+      <c r="B32" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>76</v>
+      </c>
+      <c r="B35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>80</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>87</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>96</v>
+      </c>
+      <c r="B48">
+        <v>122012</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>